<commit_message>
Fix - Update Doctors and Nurses accountAddress
</commit_message>
<xml_diff>
--- a/backend/db/daftar_aktif.xlsx
+++ b/backend/db/daftar_aktif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS Code\blockchain\skripsi\dapps-skripsi\dapps-emr-react (MAIN - LOCAL)\backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08C0B7B5-10DA-4509-BE80-50D1764F9893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E55B03A-CE1E-45F1-8567-8FDD60F1CE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{751BD174-ABD8-4C0E-B1E8-B50174B880A3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>dr. Amalia Meihati</t>
   </si>
@@ -112,13 +112,52 @@
   </si>
   <si>
     <t>Zubaidah, AMdKeb</t>
+  </si>
+  <si>
+    <t>Staf1</t>
+  </si>
+  <si>
+    <t>Staf2</t>
+  </si>
+  <si>
+    <t>0xdD76Ce44d1A22D5a3bCeD70e766AAAC95dc06f1b</t>
+  </si>
+  <si>
+    <t>0x119d6536434c434fa68CFFAFE104686a50E4Ef56</t>
+  </si>
+  <si>
+    <t>Staf</t>
+  </si>
+  <si>
+    <t>Dokter</t>
+  </si>
+  <si>
+    <t>Perawat</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>0xF3d9a8Ca72CF813C5FD1897f38C42dC726Db6A97</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>No.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,16 +165,77 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -143,14 +243,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
+    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,120 +637,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979A09FD-F336-4A26-86F4-CEC7D5E31233}">
-  <dimension ref="B2:C15"/>
+  <dimension ref="B2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="18.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F3" s="6">
+        <v>100</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="6">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="G8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="6">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="G10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="I10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="G11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="I11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="7">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="G13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="7">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="6">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="7">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="G16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="6">
+        <v>14</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="7">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="G18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
+      <c r="I18" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>